<commit_message>
Debbie is going to do stuff
</commit_message>
<xml_diff>
--- a/uploads/FLAT_2016-05_Mindgeek_Adult.xlsx
+++ b/uploads/FLAT_2016-05_Mindgeek_Adult.xlsx
@@ -3738,7 +3738,7 @@
     <t>0630614|0630614</t>
   </si>
   <si>
-    <t>Marsha May, Corinna Blake, Romi Rain</t>
+    <t>Corinna Blake, Marsha May, Romi Rain</t>
   </si>
   <si>
     <t>lesbo_massage_rubs</t>
@@ -3759,7 +3759,7 @@
     <t>0630615|0630615</t>
   </si>
   <si>
-    <t>Ash Hollywood, Juelz Ventura, Adessa Winters, Ariella Ferrera, Ava Addams, Keisha Grey, London Keyes, Jessica Jaymes</t>
+    <t>Ash Hollywood, Juelz Ventura, Adessa Winters, Ariella Ferrera, London Keyes, Jessica Jaymes, Ava Addams, Keisha Grey</t>
   </si>
   <si>
     <t>dominated_by_girls</t>
@@ -3777,7 +3777,7 @@
     <t>0630616|0630616</t>
   </si>
   <si>
-    <t>Remy LaCroix, Abby Cross, Mary Jane Mayhem, Rahyndee James, Jada Stevens, Maddy Oreilly, Kennedy Leigh</t>
+    <t>Remy LaCroix, Jada Stevens, Maddy Oreilly, Kennedy Leigh, Abby Cross, Mary Jane Mayhem, Rahyndee James</t>
   </si>
   <si>
     <t>girl_and_stepmom_gag</t>
@@ -3795,7 +3795,7 @@
     <t>0630617|0630617</t>
   </si>
   <si>
-    <t>Amanda Lane, Veronica Rayne, Bianca Breeze, Charlotte Cross, Darla Crane, Gwen Stark</t>
+    <t>Bianca Breeze, Charlotte Cross, Darla Crane, Gwen Stark, Amanda Lane, Veronica Rayne</t>
   </si>
   <si>
     <t>daughters_rough_sex</t>
@@ -3816,7 +3816,7 @@
     <t>0630618|0630618</t>
   </si>
   <si>
-    <t>Aylin Diamond, Ashley Fires, JoJo Kiss, Alessa Savage, Abigail Mac</t>
+    <t>Abigail Mac, Ashley Fires, JoJo Kiss, Alessa Savage, Aylin Diamond</t>
   </si>
   <si>
     <t>stepmom_bangs_boys</t>
@@ -3834,7 +3834,7 @@
     <t>0630619|0630619</t>
   </si>
   <si>
-    <t>Cassidy Klein, Simone Sonay, Carmel Anderson, Sensual Jane , Alexis Fawx</t>
+    <t xml:space="preserve">Alexis Fawx, Cassidy Klein, Simone Sonay, Carmel Anderson, Sensual Jane </t>
   </si>
   <si>
     <t>female_spy_punished</t>
@@ -3855,7 +3855,7 @@
     <t>0630620|0630620</t>
   </si>
   <si>
-    <t>Allie Haze, Romi Rain, Allie Haze, Peta Jensen, Romi Rain, Romi Rain</t>
+    <t>Allie Haze, Peta Jensen, Romi Rain, Allie Haze, Romi Rain, Romi Rain</t>
   </si>
   <si>
     <t>wet_nurse_creampies</t>
@@ -3873,7 +3873,7 @@
     <t>0630621|0630621</t>
   </si>
   <si>
-    <t>Peta Jensen, Kissa Sins, Pristine Edge, Isis Love</t>
+    <t>Isis Love, Peta Jensen, Kissa Sins, Pristine Edge</t>
   </si>
   <si>
     <t>asian_sex_violation</t>
@@ -3891,7 +3891,7 @@
     <t>0630622|0630622</t>
   </si>
   <si>
-    <t>Sharon Lee, Marica Hase, Jayden Lee</t>
+    <t>Marica Hase, Sharon Lee, Jayden Lee</t>
   </si>
   <si>
     <t>3way_sex_slaves</t>
@@ -3909,7 +3909,7 @@
     <t>0630623|0630623</t>
   </si>
   <si>
-    <t>Elsa Jean, Valentinna Nappi, Kimmy and Marsha Have a Threesome, Cory Chase, Billi Ann</t>
+    <t>Kimmy and Marsha Have a Threesome, Cory Chase, Billi Ann, Elsa Jean, Valentinna Nappi</t>
   </si>
   <si>
     <t>hitchhikers_suck_me</t>
@@ -3927,7 +3927,7 @@
     <t>0630624|0630624</t>
   </si>
   <si>
-    <t>Felicia Kiss, Gia Paige, Kimber Delice</t>
+    <t>Gia Paige, Kimber Delice, Felicia Kiss</t>
   </si>
   <si>
     <t>new_campus_amateurs</t>
@@ -3948,7 +3948,7 @@
     <t>0630625|0630625</t>
   </si>
   <si>
-    <t>Kimber Delice, Ryta, Daphne Klyde, Antonia Sainz</t>
+    <t>Ryta, Antonia Sainz, Kimber Delice, Daphne Klyde</t>
   </si>
   <si>
     <t>dd_homemade_breasts</t>
@@ -3969,7 +3969,7 @@
     <t>0630626|0630626</t>
   </si>
   <si>
-    <t>Cassidy Banks, Stacy Jay, Cristi Ann, Yurizan Beltran</t>
+    <t>Cassidy Banks, Yurizan Beltran, Stacy Jay, Cristi Ann</t>
   </si>
   <si>
     <t>film_me_sucking_you</t>
@@ -3990,7 +3990,7 @@
     <t>0630627|0630627</t>
   </si>
   <si>
-    <t>Lucy Doll, Brittany Shae, Lilly Sapphire, CeCe Capella</t>
+    <t>CeCe Capella, Lilly Sapphire, Lucy Doll, Brittany Shae</t>
   </si>
   <si>
     <t>girls_bang_outdoors</t>
@@ -4008,7 +4008,7 @@
     <t>0630628|0630628</t>
   </si>
   <si>
-    <t>Melissa Moore, Ally, Ava Alba</t>
+    <t>Ally, Ava Alba, Melissa Moore</t>
   </si>
   <si>
     <t>lesbian_seductions_2</t>
@@ -4029,7 +4029,7 @@
     <t>0630629|0630629</t>
   </si>
   <si>
-    <t>Lucy Li, Vinna Reed, Maci Winslett, Staci Carr, Abigail Mac, Aspen Rae, Cayla Lyons, Naomi Nevena</t>
+    <t>Abigail Mac, Aspen Rae, Cayla Lyons, Naomi Nevena, Maci Winslett, Staci Carr, Lucy Li, Vinna Reed</t>
   </si>
   <si>
     <t>dont_break_me</t>
@@ -4047,7 +4047,7 @@
     <t>0630630|0630630</t>
   </si>
   <si>
-    <t>Naomi Woods, Monica Belluci, Uma Jolie</t>
+    <t>Uma Jolie, Naomi Woods, Monica Belluci</t>
   </si>
   <si>
     <t>wives_cheat_and_choke</t>
@@ -4086,7 +4086,7 @@
     <t>0630632|0630632</t>
   </si>
   <si>
-    <t>Taylor Sands, Bianca Breeze, Ava Dalush, Aaliyah Love</t>
+    <t>Aaliyah Love, Taylor Sands, Ava Dalush, Bianca Breeze</t>
   </si>
   <si>
     <t>violated_by_cops</t>
@@ -4104,7 +4104,7 @@
     <t>0630633|0630633</t>
   </si>
   <si>
-    <t>Jessa Rhodes, Kayla Carrera, Kendra James, Dani Daniels, Kissa Sins</t>
+    <t>Kissa Sins, Dani Daniels, Jessa Rhodes, Kayla Carrera, Kendra James</t>
   </si>
   <si>
     <t>wife_and_girl_3ways</t>
@@ -4143,7 +4143,7 @@
     <t>0630635|0630635</t>
   </si>
   <si>
-    <t>Dillion Harper, August Ames, Tia Cyrus, Jean Michaels</t>
+    <t>Jean Michaels, August Ames, Dillion Harper, Tia Cyrus</t>
   </si>
   <si>
     <t>mom_sucks_off_boys</t>
@@ -4161,7 +4161,7 @@
     <t>0630636|0630636</t>
   </si>
   <si>
-    <t>Makayla Cox, Sara Jay, Richelle Ryan</t>
+    <t>Sara Jay, Makayla Cox, Richelle Ryan</t>
   </si>
   <si>
     <t>girl_boy_and_stepmom</t>
@@ -4179,7 +4179,7 @@
     <t>0630637|0630637</t>
   </si>
   <si>
-    <t>Billie Star, Abrill Gerald, Lea Lexis, Katy Rose, Leanna Sweet, Nekane</t>
+    <t>Lea Lexis, Katy Rose, Leanna Sweet, Nekane, Billie Star, Abrill Gerald</t>
   </si>
   <si>
     <t>best_of_nikki_benz</t>
@@ -4200,7 +4200,7 @@
     <t>0630638|0630638</t>
   </si>
   <si>
-    <t>Nikki Benz, Nikki Benz, Jayden Jaymes, Delta White, Nikki Benz, Nikki Sexx</t>
+    <t>Nikki Benz, Jayden Jaymes, Delta White, Nikki Benz, Nikki Benz, Nikki Sexx</t>
   </si>
   <si>
     <t>best_of_brazzers_dirty_massage</t>
@@ -4221,7 +4221,7 @@
     <t>0630639|0630639</t>
   </si>
   <si>
-    <t>Mia Malkova, Rachel Starr, Jenni Lee, Asa Akira</t>
+    <t>Rachel Starr, Jenni Lee, Asa Akira, Mia Malkova</t>
   </si>
   <si>
     <t>10_best_3somes</t>
@@ -4260,7 +4260,7 @@
     <t>0630640|0630640</t>
   </si>
   <si>
-    <t>Rachel Roxxx, Chirsty Mack, Courtney Cummz, Tasha Reign, Nikki Benz, Amy Anderssen, Madison Ivy, Monique Alexander, Brooklyn Chase, Kagney Linn Karter, Raven Bay, Rikki Six, Courtney Taylor, Summer Brielle, Keisha Grey, Mia Malkova, Brandi Love, Riley Reid, Lizz Taylor, Veronica Rodriguez</t>
+    <t>Keisha Grey, Mia Malkova, Lizz Taylor, Veronica Rodriguez, Rachel Roxxx, Chirsty Mack, Brandi Love, Riley Reid, Nikki Benz, Amy Anderssen, Courtney Taylor, Summer Brielle, Raven Bay, Rikki Six, Madison Ivy, Monique Alexander, Courtney Cummz, Tasha Reign, Brooklyn Chase, Kagney Linn Karter</t>
   </si>
   <si>
     <t>10_hottest_doctors</t>
@@ -4299,7 +4299,7 @@
     <t>0630641|0630641</t>
   </si>
   <si>
-    <t>Siri, Asa Akira, Christy Mack, Kagney Linn Karter, Bonnie Rotten, Mia Malkova, Darling Danika, Katrina Jade, Audrey Bitoni, Cherie Deville, Summer Brielle, Madison Scott, Richelle Ryan</t>
+    <t>Darling Danika, Katrina Jade, Bonnie Rotten, Mia Malkova, Audrey Bitoni, Richelle Ryan, Asa Akira, Christy Mack, Summer Brielle, Madison Scott, Kagney Linn Karter, Cherie Deville, Siri</t>
   </si>
   <si>
     <t>10_oldest_moms</t>
@@ -4338,7 +4338,7 @@
     <t>0630642|0630642</t>
   </si>
   <si>
-    <t>Tiffany Mynx, Houston, Darla Crane, Raylene, Devon, Nikita Von James, Veronica Avluv, Deauxma, Lisa Ann, Priya Anjali Rai</t>
+    <t>Darla Crane, Devon, Veronica Avluv, Priya Anjali Rai, Lisa Ann, Tiffany Mynx, Nikita Von James, Raylene, Deauxma, Houston</t>
   </si>
   <si>
     <t>10_hottest_asians</t>
@@ -4377,7 +4377,7 @@
     <t>0630643|0630643</t>
   </si>
   <si>
-    <t>Alina Li, Katsuni, Kianna Dior, Asa Akira, London Keyes, Akira Lane, Jayden Lee, Harumi Asano, Kalina Ryu, Morgan Lee, Kaylani Lei, Marica Hase</t>
+    <t>Marica Hase, Akira Lane, Katsuni, Alina Li, Jayden Lee, Harumi Asano, Kianna Dior, Asa Akira, London Keyes, Kalina Ryu, Morgan Lee, Kaylani Lei</t>
   </si>
   <si>
     <t>gay_dirty_uncle_dennis</t>
@@ -4398,7 +4398,7 @@
     <t>0630656|0630656</t>
   </si>
   <si>
-    <t>Dennis West, Luke Adams, Will Braun, Dennis West, Scott Riley, Alex Mecum, Dennis West, Dennis West, Landon Mycles</t>
+    <t>Alex Mecum, Dennis West, Dennis West, Luke Adams, Will Braun, Dennis West, Landon Mycles, Dennis West, Scott Riley</t>
   </si>
   <si>
     <t>gay_milked_by_hot_men</t>
@@ -4419,7 +4419,7 @@
     <t>0630657|0630657</t>
   </si>
   <si>
-    <t>Jimmy Fanz, Phenix Saint, Phenix Saint, Scott Riley, Phenix Saint, Tommy Regan, Dennis West, Jake Bass</t>
+    <t>Phenix Saint, Tommy Regan, Dennis West, Jake Bass, Phenix Saint, Scott Riley, Jimmy Fanz, Phenix Saint</t>
   </si>
   <si>
     <t>gay_first_prison_sex</t>
@@ -4440,7 +4440,7 @@
     <t>0630658|0630658</t>
   </si>
   <si>
-    <t>Landon Mycles, Sebastian Young, Adam Bryant, Josh Peters, Dimitri Kane, Tony Paradise, Blue Moores, Paddy O'Brian</t>
+    <t>Blue Moores, Paddy O'Brian, Dimitri Kane, Tony Paradise, Landon Mycles, Sebastian Young, Adam Bryant, Josh Peters</t>
   </si>
   <si>
     <t>gay_athletic_boys_bang</t>
@@ -4461,7 +4461,7 @@
     <t>0630659|0630659</t>
   </si>
   <si>
-    <t>Damien Michaels, Jordan Boss, Luke Adams, Will Braun, Peter Fields, Will Braun, Josh Peters, Will Braun</t>
+    <t>Peter Fields, Will Braun, Luke Adams, Will Braun, Damien Michaels, Jordan Boss, Josh Peters, Will Braun</t>
   </si>
   <si>
     <t>gay_secret_cult_orgys</t>
@@ -4482,7 +4482,7 @@
     <t>0630660|0630660</t>
   </si>
   <si>
-    <t>Jack Hunter, Will Braun, Colby Keller, Roman Todd, Addison Graham, Brandon Moore, Colby Keller, Roman Todd, Will Braun, Colby Keller, Will Braun</t>
+    <t>Jack Hunter, Will Braun, Colby Keller, Will Braun, Colby Keller, Roman Todd, Addison Graham, Brandon Moore, Colby Keller, Roman Todd, Will Braun</t>
   </si>
   <si>
     <t>gay_hot_men_of_new_york</t>
@@ -4503,7 +4503,7 @@
     <t>0630661|0630661</t>
   </si>
   <si>
-    <t>Diego Sans, Ricky Decker, Bennett Anthony, Roman Todd, Diego Sans, Scott Riley, Diego Sans, Jordan Boss</t>
+    <t>Diego Sans, Jordan Boss, Diego Sans, Ricky Decker, Bennett Anthony, Roman Todd, Diego Sans, Scott Riley</t>
   </si>
   <si>
     <t>gay_truck_stop_hookups</t>
@@ -4524,7 +4524,7 @@
     <t>0630662|0630662</t>
   </si>
   <si>
-    <t>Colby Jansen, Dario Beck, Dario Beck, Massimo Piano, Damien Crosse, Dario Beck, JJ Knight, Tommy Regan</t>
+    <t>Damien Crosse, Dario Beck, Colby Jansen, Dario Beck, Dario Beck, Massimo Piano, JJ Knight, Tommy Regan</t>
   </si>
   <si>
     <t>gay_addicted_to_spunk</t>
@@ -4545,7 +4545,7 @@
     <t>0630663|0630663</t>
   </si>
   <si>
-    <t>Alex Mecum, Colby Keller, Bruno Bernal, Jake Bass, Alex Mecum, Aspen, Klein Kerr, Massimo Piano</t>
+    <t>Alex Mecum, Aspen, Klein Kerr, Massimo Piano, Bruno Bernal, Jake Bass, Alex Mecum, Colby Keller</t>
   </si>
   <si>
     <t>gay_10_best_doms</t>
@@ -4584,7 +4584,7 @@
     <t>0630664|0630664</t>
   </si>
   <si>
-    <t>Boston Miles, Johnny Rapid, Travis Irons , Dereck Fox, Tyler St.James, Adam Killian, Trenton Ducati, Christian Wilde, Cliff Jensen, Gavin Waters, Phillip Aubrey, Colby Jansen, Duncan Black, Johnny Rapid, Sebastian Young, Adam Killian, John Magnum, Parker London, Phenix Saint, Sebastian Keys, Tony Paradise, Rafael Alencar, Johnny Rapid, Spencer Fox, Colby Keller, Jake Steel</t>
+    <t>Adam Killian, John Magnum, Johnny Rapid, Sebastian Young, Christian Wilde, Cliff Jensen, Gavin Waters, Phillip Aubrey, Adam Killian, Trenton Ducati, Colby Keller, Jake Steel, Dereck Fox, Tyler St.James, Boston Miles, Johnny Rapid, Travis Irons , Colby Jansen, Duncan Black, Parker London, Phenix Saint, Sebastian Keys, Tony Paradise, Rafael Alencar, Johnny Rapid, Spencer Fox</t>
   </si>
   <si>
     <t>Scene Only</t>
@@ -4764,7 +4764,7 @@
     <t>media_sourced_from</t>
   </si>
   <si>
-    <t>02/18/2016 03:08:27</t>
+    <t>02/18/2016 10:29:32</t>
   </si>
 </sst>
 </file>

</xml_diff>